<commit_message>
Torsdag d. 14. marts kl.12
Litteratursøgning - abstract
</commit_message>
<xml_diff>
--- a/Liste over litteratur.xlsx
+++ b/Liste over litteratur.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kirstine/Documents/GitHub/Bachelor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77A126D9-5F8C-B447-AC54-B51694BBBBE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47C9520-D058-5645-911F-5AA6F27F8448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="16100" xr2:uid="{733265EB-9D21-354D-94CD-9E52C4EF0070}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{733265EB-9D21-354D-94CD-9E52C4EF0070}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="144">
   <si>
     <t>Navn</t>
   </si>
@@ -53,10 +53,421 @@
     <t>Titel</t>
   </si>
   <si>
-    <t>chrome-extension://efaidnbmnnnibpcajpcglclefindmkaj/https://art.torvergata.it/bitstream/2108/303883/1/aer.20190623.pdf</t>
-  </si>
-  <si>
     <t># Citater</t>
+  </si>
+  <si>
+    <t>Asker et al. (2021)</t>
+  </si>
+  <si>
+    <t>ARTIFICIAL INTELLIGENCE AND PRICING: THE IMPACT OF ALGORITHM DESIGN</t>
+  </si>
+  <si>
+    <t>https://www.nber.org/papers/w28535</t>
+  </si>
+  <si>
+    <t>Asynkron og synkron learning</t>
+  </si>
+  <si>
+    <t>Algorithmic Pricing and Competition:Empirical Evidence from the GermanRetail Gasoline Market</t>
+  </si>
+  <si>
+    <t>https://www.journals.uchicago.edu/doi/epdf/10.1086/726906</t>
+  </si>
+  <si>
+    <t>Introduktion - empirisk</t>
+  </si>
+  <si>
+    <t>Assad et al. (2024)</t>
+  </si>
+  <si>
+    <t>chrome-extension://efaidnbmnnnibpcajpcglclefindmkaj/https://citeseerx.ist.psu.edu/document?repid=rep1&amp;type=pdf&amp;doi=86cd466320d6f0a0243798ceed1a3d8b28fc53aa</t>
+  </si>
+  <si>
+    <t>Bowling &amp; Veloso (2001)</t>
+  </si>
+  <si>
+    <t>Rational and Convergent Learning in Stochastic Games</t>
+  </si>
+  <si>
+    <t>Stokastisk spil. Siger noget om Wolf</t>
+  </si>
+  <si>
+    <t>Bowling &amp; Veloso (2002)</t>
+  </si>
+  <si>
+    <t>Multiagent learning using a variable learning rate</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0004370202001212</t>
+  </si>
+  <si>
+    <t>A Comprehensive Survey of Multiagent Reinforcement Learning</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/4445757</t>
+  </si>
+  <si>
+    <t>Rigtig god for forståelsen af MARL</t>
+  </si>
+  <si>
+    <t>Busoniu et al. (2008)</t>
+  </si>
+  <si>
+    <t>Busoniu et al. (2010)</t>
+  </si>
+  <si>
+    <t>Multi-agent Reinforcement Learning: An Overview</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/chapter/10.1007/978-3-642-14435-6_7</t>
+  </si>
+  <si>
+    <t>Rigtig god for forståelsen af MARL. Indeholder måske ideer til yderligere undersøgelser</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence, Algorithmic Pricing, and Collusion</t>
+  </si>
+  <si>
+    <t>Calvano et al. (2020)</t>
+  </si>
+  <si>
+    <t>https://www.aeaweb.org/articles?id=10.1257/aer.20190623</t>
+  </si>
+  <si>
+    <t>SKAL LÆSES. Ændringer i efterspørgsel, omkostning og antal spillere. Figur om delta</t>
+  </si>
+  <si>
+    <t>An Empirical Analysis of Algorithmic Pricing on Amazon Marketplace</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/abs/10.1145/2872427.2883089</t>
+  </si>
+  <si>
+    <t>Empirisk om Amazon marketplace</t>
+  </si>
+  <si>
+    <t>Chen et al. (2016)</t>
+  </si>
+  <si>
+    <t>Either with us or against us: experimental evidence on partial cartels</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/s11238-021-09842-z</t>
+  </si>
+  <si>
+    <t>Clemens &amp; Rau (2022)</t>
+  </si>
+  <si>
+    <t>Partial cartel og kommunikation. Julius bruger den i forbindelse med Edgeworth cycles</t>
+  </si>
+  <si>
+    <t>Learning to compete, coordinate, and cooperate in repeated games using reinforcement learning</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/s10994-010-5192-9</t>
+  </si>
+  <si>
+    <t>Crandall &amp; Goodrich (2011)</t>
+  </si>
+  <si>
+    <t>Mulig anden algoritme: M-Qubed. Julius afviser denne. Det er en anden måde at initialisere Q-tabeller</t>
+  </si>
+  <si>
+    <t>Investigating the Impact of Direct Punishment on the Emergence of Cooperation in Multi-Agent Reinforcement Learning Systems</t>
+  </si>
+  <si>
+    <t>Dasgupta &amp; Musolesi (2023)</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2301.08278</t>
+  </si>
+  <si>
+    <t>Julius bruger denne i diskussionen. Punishment</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/abs/10.1145/1160633.1160770</t>
+  </si>
+  <si>
+    <t>de Cote et al. (2006)</t>
+  </si>
+  <si>
+    <t>Learning to cooperate in multi-agent social dilemmas</t>
+  </si>
+  <si>
+    <t>Forskellige principper: Change or Learn Fast and Change and Keep: Q-tables bliver initialiseret anderledes</t>
+  </si>
+  <si>
+    <t>Ezrachi &amp; Stucke (2015)</t>
+  </si>
+  <si>
+    <t>https://heinonline.org/HOL/Page?handle=hein.journals/unilllr2017&amp;div=59&amp;g_sent=1&amp;casa_token=&amp;collection=journals</t>
+  </si>
+  <si>
+    <t>ARTIFICIAL INTELLIGENCE COLLUSION: WHEN COMPUTERS INHIBIT COMPETITION</t>
+  </si>
+  <si>
+    <t>Etik og lov. Forudsigelig agent (Julius)</t>
+  </si>
+  <si>
+    <t>Learning with Opponent-Learning Awareness</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/1709.04326</t>
+  </si>
+  <si>
+    <t>Deep MARL - LOLA</t>
+  </si>
+  <si>
+    <t>Foerster et al. (2017)</t>
+  </si>
+  <si>
+    <t>Correlated-Q Learning.</t>
+  </si>
+  <si>
+    <t>chrome-extension://efaidnbmnnnibpcajpcglclefindmkaj/https://cdn.aaai.org/Symposia/Spring/2002/SS-02-02/SS02-02-012.pdf</t>
+  </si>
+  <si>
+    <t>Julius bruger denne i diskussionen. Fuld kendskab</t>
+  </si>
+  <si>
+    <t>Greenwald &amp; Hall (2003)</t>
+  </si>
+  <si>
+    <t>Julius bruger denne i diskussionen. Peer evaluation</t>
+  </si>
+  <si>
+    <t>chrome-extension://efaidnbmnnnibpcajpcglclefindmkaj/https://ifaamas.org/Proceedings/aamas2020/pdfs/p520.pdf</t>
+  </si>
+  <si>
+    <t>Hostallero et al. (2020)</t>
+  </si>
+  <si>
+    <t>Inducing Cooperation through Reward Reshaping Based on Peer Evaluations in Deep Multi-Agent Reinforcement Learning.</t>
+  </si>
+  <si>
+    <t>Dynamic programming and Markov processes</t>
+  </si>
+  <si>
+    <t>Julius bruger den til klassifikation</t>
+  </si>
+  <si>
+    <t>https://psycnet.apa.org/record/1961-01474-000</t>
+  </si>
+  <si>
+    <t>Howard (1960)</t>
+  </si>
+  <si>
+    <t>Hu &amp; Wellman (2003)</t>
+  </si>
+  <si>
+    <t>chrome-extension://efaidnbmnnnibpcajpcglclefindmkaj/https://www.jmlr.org/papers/volume4/temp/hu03a.pdf</t>
+  </si>
+  <si>
+    <t>Nash Q-Learning for General-Sum Stochastic Games</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Julius afviser denne: komplet information. Anden algoritme: Nash-Q. </t>
+  </si>
+  <si>
+    <t>Klein</t>
+  </si>
+  <si>
+    <t>Autonomous Algorithmic Collusion: Q-learning under Sequential Pricing</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/full/10.1111/1756-2171.12383</t>
+  </si>
+  <si>
+    <t>Klein (2021)</t>
+  </si>
+  <si>
+    <t>Friend-or-Foe Q-Learning in General-Sum Games</t>
+  </si>
+  <si>
+    <t>Littman (2001)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Julius afviser denne: komplet information. Anden algoritme: FFQ </t>
+  </si>
+  <si>
+    <t>chrome-extension://efaidnbmnnnibpcajpcglclefindmkaj/https://www.researchgate.net/profile/Michael-Littman/publication/2933305_Friend-or-Foe_Q-learning_in_General-Sum_Games/links/54b66cb80cf24eb34f6d19dc/Friend-or-Foe-Q-learning-in-General-Sum-Games.pdf</t>
+  </si>
+  <si>
+    <t>International Journal of Computational Intelligence Systems</t>
+  </si>
+  <si>
+    <t>https://www.atlantis-press.com/journals/ijcis/125957073/view</t>
+  </si>
+  <si>
+    <t>Liu &amp; Jia (2021)</t>
+  </si>
+  <si>
+    <t>Stokastisk spil. Regret minimization. Julius bruger denne til at forklare agent-environment interaction in a markov game. Forståelse</t>
+  </si>
+  <si>
+    <t>Multi-Agent Actor-Critic for Mixed Cooperative-Competitive Environments</t>
+  </si>
+  <si>
+    <t>https://proceedings.neurips.cc/paper/2017/hash/68a9750337a418a86fe06c1991a1d64c-Abstract.html</t>
+  </si>
+  <si>
+    <t>Lowe et al. (2017)</t>
+  </si>
+  <si>
+    <t>Deep MARL - Julius bruger denne i diskussionen. Q-learning kritieres. Mulige andre policies</t>
+  </si>
+  <si>
+    <t>Maskin &amp; Tirole (1988)</t>
+  </si>
+  <si>
+    <t>https://www.jstor.org/stable/1911701</t>
+  </si>
+  <si>
+    <t>A Theory of Dynamic Oligopoly, II: Price Competition, Kinked Demand Curves, and Edgeworth Cycles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kan bruges til teorien - Edgeworth cycle og sequential model </t>
+  </si>
+  <si>
+    <t>Matignon et al. (2012)</t>
+  </si>
+  <si>
+    <t>Independent reinforcement learners in cooperative Markov games: a survey regarding coordination problems</t>
+  </si>
+  <si>
+    <t>https://www.cambridge.org/core/journals/knowledge-engineering-review/article/independent-reinforcement-learners-in-cooperative-markov-games-a-survey-regarding-coordination-problems/05C8A9CB66528DA19B855B8C5DFBA981</t>
+  </si>
+  <si>
+    <t>Mulige andre tilgange og policies</t>
+  </si>
+  <si>
+    <t>Game Theory and Multi-agent Reinforcement Learning</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/chapter/10.1007/978-3-642-27645-3_14</t>
+  </si>
+  <si>
+    <t>Nowé et al. (2012)</t>
+  </si>
+  <si>
+    <t>Multiagent reinforcement learning in the Iterated Prisoner's Dilemma</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/0303264795015515</t>
+  </si>
+  <si>
+    <t>Sandholm &amp; Crites (1996)</t>
+  </si>
+  <si>
+    <t>longer exploration in IPD - gør det sig gældende andre steder?</t>
+  </si>
+  <si>
+    <t>Learning To Cooperate in a Social Dilemma: A Satisficing Approach to Bargaining</t>
+  </si>
+  <si>
+    <t>chrome-extension://efaidnbmnnnibpcajpcglclefindmkaj/https://cdn.aaai.org/ICML/2003/ICML03-095.pdf</t>
+  </si>
+  <si>
+    <t>Bruger mere end to agenter. Mulig princip: Give-and-take</t>
+  </si>
+  <si>
+    <t>Stimpson &amp; Goodrich (2003)</t>
+  </si>
+  <si>
+    <t>Stimpson et al. (2001)</t>
+  </si>
+  <si>
+    <t>chrome-extension://efaidnbmnnnibpcajpcglclefindmkaj/https://faculty.cs.byu.edu/~mike/mikeg/papers/IJCAI.pdf</t>
+  </si>
+  <si>
+    <t>Satisficing and Learning Cooperation in the Prisoner’s Dilemma.</t>
+  </si>
+  <si>
+    <t>Initialisering af Q-tables</t>
+  </si>
+  <si>
+    <t>Reinforcement Learning: An Introduction (Second ed.)</t>
+  </si>
+  <si>
+    <t>https://books.google.dk/books?hl=da&amp;lr=&amp;id=uWV0DwAAQBAJ&amp;oi=fnd&amp;pg=PR7&amp;dq=Sutton,+R.+S.+and+A.+G.+Barto+(2018).+Reinforcement+Learning:+An+Introduction+(Second+ed.).&amp;ots=mjoEq720i2&amp;sig=x9Cl519GGJJKUpDONXkDc3Mc8tI&amp;redir_esc=y - v=onepage&amp;q=Sutton, R. S. and A. G. Barto (2018). Reinforcement Learning%3A An Introduction (Second ed.).&amp;f=false</t>
+  </si>
+  <si>
+    <t>Kan bruges til teorien. Måske er der noget om policies også</t>
+  </si>
+  <si>
+    <t>Sutton &amp; Barto (2018)</t>
+  </si>
+  <si>
+    <t>https://proceedings.neurips.cc/paper_files/paper/1999/hash/464d828b85b0bed98e80ade0a5c43b0f-Abstract.html</t>
+  </si>
+  <si>
+    <t>Sutton et al. (1999)</t>
+  </si>
+  <si>
+    <t>Policy-gradient</t>
+  </si>
+  <si>
+    <t>Policy Gradient Methods for Reinforcement Learning with Function Approximation</t>
+  </si>
+  <si>
+    <t>Waltman &amp; Kaymak (2008)</t>
+  </si>
+  <si>
+    <t>Q-learning agents in a Cournot oligopoly model</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0165188908000183</t>
+  </si>
+  <si>
+    <t>Cournot. Simultant spil</t>
+  </si>
+  <si>
+    <t>Q-learning</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/bf00992698</t>
+  </si>
+  <si>
+    <t>Watkins &amp; Dayan (1992)</t>
+  </si>
+  <si>
+    <t>Stationarity og convergence. Til teorien og forståelse (convergence)</t>
+  </si>
+  <si>
+    <t>Invention of Q-learning</t>
+  </si>
+  <si>
+    <t>chrome-extension://efaidnbmnnnibpcajpcglclefindmkaj/https://d1wqtxts1xzle7.cloudfront.net/50360235/Learning_from_delayed_rewards_20161116-28282-v2pwvq-libre.pdf?1479337768=&amp;response-content-disposition=inline%3B+filename=Learning_from_delayed_rewards.pdf&amp;Expires=1710416375&amp;Signature=Y7d20DFmoeFnIeMLkA0HAqYfEOXzgrjdEjrJ-A9Xd94XL3bbA3KtdohWIn2uUJNScnUreBtf-M~lFSRb8PlbtOPZd8H~EWnhM20YDdszqj6RtZRD0LE-aQ7erHZR6O-aYR483ZPruA2uKfmlN931Ow8Gaog4~PXYXCxDzLll57hOdBJSIWLIXkuEz-znl8WgvhErSDqg9-QHcvb8fA5YRYrpHNkRtegf8WN7-rcsubklnQKHjpIDCTwhtR4y9AXiuXY1vgALg0OnBu6MlQYw8TBsSWCBj25SfJlHx-ZdbrlC6esrgXpmjjNB7HxdLmUAF8zDrWusOU393V~ztb3woQ__&amp;Key-Pair-Id=APKAJLOHF5GGSLRBV4ZA</t>
+  </si>
+  <si>
+    <t>Learning From Delayed Rewards.</t>
+  </si>
+  <si>
+    <t>Watkins (1989)</t>
+  </si>
+  <si>
+    <t>Learning Zero-Sum Simultaneous-Move Markov Games Using Function Approximation and Correlated Equilibrium</t>
+  </si>
+  <si>
+    <t>Der findes en nyere artikel - denne er måske mere brugbar</t>
+  </si>
+  <si>
+    <t>Xie et al. (2020)</t>
+  </si>
+  <si>
+    <t>https://proceedings.mlr.press/v125/xie20a.html</t>
+  </si>
+  <si>
+    <t>Multi-Agent Reinforcement Learning: A Selective Overview of Theories and Algorithms</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/chapter/10.1007/978-3-030-60990-0_12</t>
+  </si>
+  <si>
+    <t>Zhang et al. (2021)</t>
+  </si>
+  <si>
+    <t>Kan være relevant for teorien. Policy-based methods - mulige tilgange</t>
   </si>
 </sst>
 </file>
@@ -86,12 +497,24 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -107,16 +530,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -145,14 +605,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{10176270-C728-234C-A5E7-77C9B6C878C2}" name="Tabel1" displayName="Tabel1" ref="A1:F223" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{10176270-C728-234C-A5E7-77C9B6C878C2}" name="Tabel1" displayName="Tabel1" ref="A1:F223" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:F223" xr:uid="{10176270-C728-234C-A5E7-77C9B6C878C2}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{1166767B-C3A8-6F47-B004-E3D9E1AAC2B9}" name="Navn"/>
     <tableColumn id="2" xr3:uid="{55BE3EDC-57A3-6042-915C-CBE889552E90}" name="Link"/>
     <tableColumn id="3" xr3:uid="{430447A9-979A-6F41-80F9-C1949336AD14}" name="Titel"/>
-    <tableColumn id="4" xr3:uid="{4E0B886A-F6FD-A242-AD55-C10C60DA5D47}" name="Stjerner"/>
-    <tableColumn id="5" xr3:uid="{1C361871-60F3-1F46-935D-F813791A35C5}" name="Stikord"/>
+    <tableColumn id="4" xr3:uid="{4E0B886A-F6FD-A242-AD55-C10C60DA5D47}" name="Stjerner" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{1C361871-60F3-1F46-935D-F813791A35C5}" name="Stikord" dataDxfId="1"/>
     <tableColumn id="8" xr3:uid="{14E1A955-0C73-6341-A5FB-F5576A2310C1}" name="# Citater"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -456,17 +916,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42231D9-A03D-254A-930A-A47BD9C59C00}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="107.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="11" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="145.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="109.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="11" customWidth="1"/>
+    <col min="5" max="5" width="110.6640625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -479,28 +941,759 @@
       <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="11">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="11">
         <v>5</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="11">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="11">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="11">
+        <v>5</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6">
+        <v>2668</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="12">
+        <v>5</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="11">
+        <v>4</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="11">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="11">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="11">
+        <v>4</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="11">
+        <v>1</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="11">
+        <v>4</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="11">
+        <v>1</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="11">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="11">
+        <v>1</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="11">
+        <v>1</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="11">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18">
+        <v>6362</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="11">
+        <v>2</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19">
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="12">
+        <v>5</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="11">
+        <v>2</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21" s="7">
+        <v>914</v>
+      </c>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="11">
+        <v>2</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="13">
+        <v>4</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F23">
+        <v>4398</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" s="11">
+        <v>5</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F24">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" s="12">
+        <v>5</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F25" s="7">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" s="12">
+        <v>5</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F26">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" t="s">
+        <v>104</v>
+      </c>
+      <c r="D27" s="12">
+        <v>5</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" t="s">
+        <v>108</v>
+      </c>
+      <c r="D28" s="11">
+        <v>3</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F28">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="11">
+        <v>3</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F29">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D30" s="11">
+        <v>5</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F30" s="7">
+        <v>69009</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>121</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" s="11">
+        <v>1</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="F31">
+        <v>7956</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" t="s">
+        <v>125</v>
+      </c>
+      <c r="D32" s="11">
+        <v>1</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F32">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>130</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" t="s">
+        <v>128</v>
+      </c>
+      <c r="D33" s="11">
+        <v>4</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F33">
+        <v>18499</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="119" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" s="11">
+        <v>4</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="F34" s="7">
+        <v>9902</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>138</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C35" t="s">
+        <v>136</v>
+      </c>
+      <c r="D35" s="11">
+        <v>4</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F35">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>142</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C36" t="s">
+        <v>140</v>
+      </c>
+      <c r="D36" s="13">
+        <v>4</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F36">
+        <v>1174</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{4D6E6AC7-127A-1B4C-BC1F-DB196428AE97}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{35538D25-3178-104D-A704-903311D84543}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{FF5F8F2B-D394-6241-A41D-B706550713F2}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{9E03EB3C-4D4A-634B-8FA6-76796E27C2F0}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{15781122-A6AD-F545-B27F-F205090AFE0A}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{8E88F00A-FD91-724E-AD95-4052ED5B7405}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{5916307F-77C7-6E49-B8EB-DAEB1A3827E4}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{69248453-50E1-B04F-A080-4B5FB20AAC7B}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{243CC3D7-A416-794E-AF7A-E64FE0AD25C1}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{D42CB2B2-7778-2F40-8BBF-80D993B12ADE}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{9E6C0495-1053-734B-AC77-CC9CF3A06DF2}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{55772CE3-91E5-C048-9401-5EC11075A9F3}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{62745E2C-E83C-3747-A648-4DC2C1E064DB}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{3722C7CB-3B31-4546-BB0C-4A0557879DB4}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{FC1DE14C-170B-D344-80CF-AFD9F4B52D19}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{445BD09D-5796-184A-93B2-B663060B378B}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{AFCB1253-2F35-1848-9BCC-88C793ACCF13}"/>
+    <hyperlink ref="B18" r:id="rId17" xr:uid="{D5AA4A38-F752-FE4B-9191-AF879B55F975}"/>
+    <hyperlink ref="B20" r:id="rId18" xr:uid="{CBFE1A5E-75D9-F04B-A8C8-026151DA65D3}"/>
+    <hyperlink ref="B21" r:id="rId19" xr:uid="{67A76FA8-F4A0-A44F-9FE7-C379D208F1CF}"/>
+    <hyperlink ref="B22" r:id="rId20" xr:uid="{374B59A7-A240-094F-9958-ED4934A50227}"/>
+    <hyperlink ref="B23" r:id="rId21" xr:uid="{968AF659-6ABA-5449-B321-85C9730DF463}"/>
+    <hyperlink ref="B24" r:id="rId22" xr:uid="{F6E011E6-BF7B-7A42-B82D-FFC7BB303179}"/>
+    <hyperlink ref="B25" r:id="rId23" xr:uid="{5C694919-353A-3541-B144-81172BA584FF}"/>
+    <hyperlink ref="B26" r:id="rId24" xr:uid="{7B2EADBE-BE4A-2B47-815A-57C8C28F63F1}"/>
+    <hyperlink ref="B27" r:id="rId25" xr:uid="{9990DBE7-0045-244E-A1E9-6286F2C0EF43}"/>
+    <hyperlink ref="B28" r:id="rId26" xr:uid="{A18686C5-F3A5-D044-A7F9-187D33B3BCD3}"/>
+    <hyperlink ref="B29" r:id="rId27" xr:uid="{53BA460E-898A-3A49-A074-9E082E89B0BD}"/>
+    <hyperlink ref="B30" r:id="rId28" location="v=onepage&amp;q=Sutton%2C%20R.%20S.%20and%20A.%20G.%20Barto%20(2018).%20Reinforcement%20Learning%3A%20An%20Introduction%20(Second%20ed.).&amp;f=false" display="https://books.google.dk/books?hl=da&amp;lr=&amp;id=uWV0DwAAQBAJ&amp;oi=fnd&amp;pg=PR7&amp;dq=Sutton,+R.+S.+and+A.+G.+Barto+(2018).+Reinforcement+Learning:+An+Introduction+(Second+ed.).&amp;ots=mjoEq720i2&amp;sig=x9Cl519GGJJKUpDONXkDc3Mc8tI&amp;redir_esc=y - v=onepage&amp;q=Sutton, R. S. and A. G. Barto (2018). Reinforcement Learning%3A An Introduction (Second ed.).&amp;f=false" xr:uid="{DA058FA0-9E40-A646-A212-EEC9C56C408B}"/>
+    <hyperlink ref="B31" r:id="rId29" xr:uid="{9716592F-948D-C148-9CAE-BBF0C63C5E92}"/>
+    <hyperlink ref="B32" r:id="rId30" xr:uid="{06DB60D1-BD93-8D4B-8E03-65BA56C98029}"/>
+    <hyperlink ref="B34" r:id="rId31" display="chrome-extension://efaidnbmnnnibpcajpcglclefindmkaj/https://d1wqtxts1xzle7.cloudfront.net/50360235/Learning_from_delayed_rewards_20161116-28282-v2pwvq-libre.pdf?1479337768=&amp;response-content-disposition=inline%3B+filename=Learning_from_delayed_rewards.pdf&amp;Expires=1710416375&amp;Signature=Y7d20DFmoeFnIeMLkA0HAqYfEOXzgrjdEjrJ-A9Xd94XL3bbA3KtdohWIn2uUJNScnUreBtf-M~lFSRb8PlbtOPZd8H~EWnhM20YDdszqj6RtZRD0LE-aQ7erHZR6O-aYR483ZPruA2uKfmlN931Ow8Gaog4~PXYXCxDzLll57hOdBJSIWLIXkuEz-znl8WgvhErSDqg9-QHcvb8fA5YRYrpHNkRtegf8WN7-rcsubklnQKHjpIDCTwhtR4y9AXiuXY1vgALg0OnBu6MlQYw8TBsSWCBj25SfJlHx-ZdbrlC6esrgXpmjjNB7HxdLmUAF8zDrWusOU393V~ztb3woQ__&amp;Key-Pair-Id=APKAJLOHF5GGSLRBV4ZA" xr:uid="{6017713B-9B01-DE40-B220-6DA457A78EE7}"/>
+    <hyperlink ref="B35" r:id="rId32" xr:uid="{C2CE98E4-0AAD-454D-A001-3AA782BD7891}"/>
+    <hyperlink ref="B36" r:id="rId33" xr:uid="{7BBC9801-BB86-804A-B00D-C0B096AAB344}"/>
+    <hyperlink ref="B19" r:id="rId34" xr:uid="{F49D9848-C025-4E4B-8130-BF1458B8AB06}"/>
+    <hyperlink ref="B33" r:id="rId35" xr:uid="{0FF38B02-4E7E-CD45-A6AB-35D62F26978B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId36"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lørdag d. 16. marts
Lørdag d. 16. marts
</commit_message>
<xml_diff>
--- a/Liste over litteratur.xlsx
+++ b/Liste over litteratur.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kirstine/Documents/GitHub/Bachelor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47C9520-D058-5645-911F-5AA6F27F8448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0186870C-82E5-1B41-845F-EE38214420A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{733265EB-9D21-354D-94CD-9E52C4EF0070}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="180">
   <si>
     <t>Navn</t>
   </si>
@@ -468,6 +468,114 @@
   </si>
   <si>
     <t>Kan være relevant for teorien. Policy-based methods - mulige tilgange</t>
+  </si>
+  <si>
+    <t>chrome-extension://efaidnbmnnnibpcajpcglclefindmkaj/https://research.tue.nl/files/46220362/SSCI16_paper_737.pdf</t>
+  </si>
+  <si>
+    <t>Comparing exploration strategies for Q-learning in random stochastic mazes</t>
+  </si>
+  <si>
+    <t>Tijsma et al. (2017)</t>
+  </si>
+  <si>
+    <t>Explorations in Reinforcement Learning: Online Action Selection and Value Function Approximation</t>
+  </si>
+  <si>
+    <t>chrome-extension://efaidnbmnnnibpcajpcglclefindmkaj/https://www.researchgate.net/profile/Saba-Yahyaa/publication/276904847_Explorations_in_Reinforcement_Learning_Online_Action_Selection_and_Value_Function_Approximation/links/555b2ea408ae6943a8793fe3/Explorations-in-Reinforcement-Learning-Online-Action-Selection-and-Value-Function-Approximation.pdf</t>
+  </si>
+  <si>
+    <t>Saba (2015)</t>
+  </si>
+  <si>
+    <t>Nævner forskellige brugbare policies</t>
+  </si>
+  <si>
+    <t>Multi-armed Bandit Algorithms and Empirical Evaluation</t>
+  </si>
+  <si>
+    <t>Single-agent - Maze? Kan være relevant at teste de forskellige selections i vores multi-agent. Epsilon-greedy er den værste</t>
+  </si>
+  <si>
+    <t>MAB. Epsilon-greedy er den bedste</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/chapter/10.1007/11564096_42</t>
+  </si>
+  <si>
+    <t>Vermorel &amp; Mohri (2005)</t>
+  </si>
+  <si>
+    <t>A new Q-learning algorithm based on the metropolis criterion</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/1335509?casa_token=55KVTt3z1FYAAAAA:fJFkz6DUMbYv3IWNHYFECSRCdX_qR2WgNkUpAEWZtOik5ryLgeJ-HwRDPyD0v0JNgqsbsFmhajDCSQ&amp;fbclid=IwAR3Q416BXN_PBaoBGKpoQeoxto7RIT4UMhQMNHOB-9_uef-skfAzYt_s5Qk</t>
+  </si>
+  <si>
+    <t>Guo (2004)</t>
+  </si>
+  <si>
+    <t>SA-Q-Learnong, Boltzmann. Puzzle-problem</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/chapter/10.1007/978-3-030-31978-6_11?fbclid=IwAR3nHtiunDuxVRdefETKGj2vgOyhr0K-Y0X4CMlt4LS4iAOcAKoXl9BRRUs - Equ3</t>
+  </si>
+  <si>
+    <t>Sammenligner epsilon med dynamic epsilon</t>
+  </si>
+  <si>
+    <t>Assessing the Potential of Classical Q-learning in General Game Playing</t>
+  </si>
+  <si>
+    <t>Wang (2019)</t>
+  </si>
+  <si>
+    <t>https://proceedings.neurips.cc/paper_files/paper/2001/file/6f2688a5fce7d48c8d19762b88c32c3b-Paper.pdf</t>
+  </si>
+  <si>
+    <t>Basic viden om dynamic epsilon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convergence of Optimistic and Incremental Q-Learning </t>
+  </si>
+  <si>
+    <t>Even-Dar &amp; Mansour (2001)</t>
+  </si>
+  <si>
+    <t>chrome-extension://efaidnbmnnnibpcajpcglclefindmkaj/https://arxiv.org/pdf/2007.00869.pdf</t>
+  </si>
+  <si>
+    <t>ε-BMC: ABayesian Ensemble Approach to Epsilon-Greedy Exploration in Model-Free Reinforcement Learning</t>
+  </si>
+  <si>
+    <t>Gimelfarb et al. (2020)</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/chapter/10.1007/978-3-642-24455-1_33</t>
+  </si>
+  <si>
+    <t>Value-Difference Based Exploration: Adaptive Control between Epsilon-Greedy and Softmax</t>
+  </si>
+  <si>
+    <t>Tokic &amp; Palm (2011)</t>
+  </si>
+  <si>
+    <t>Sammenligner VDBE-SoftMax med epsilon. Bruger pure epsilon-greedy</t>
+  </si>
+  <si>
+    <t>Sammenligner epsilon med epsilon-BMC. Bruger pure epsilon-greedy og argumenterer for brug af dette. I vores scenarie vil vi ikke bruge pure epsilon-greedy</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/s12597-012-0077-2?fbclid=IwAR3enZoej3vH2xP5mrisHdfml-3CLnaaEdiPx5Os7UjMmM4ELceobu1fbQE</t>
+  </si>
+  <si>
+    <t>Reinforcement learning: exploration–exploitation dilemma in multi-agent foraging task</t>
+  </si>
+  <si>
+    <t>Sammenligner forskellige policies i robot setting?</t>
+  </si>
+  <si>
+    <t>Yogeswaran &amp; Ponnambalam (2012)</t>
   </si>
 </sst>
 </file>
@@ -540,7 +648,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -549,9 +656,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -565,6 +669,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -572,10 +682,10 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -611,8 +721,8 @@
     <tableColumn id="1" xr3:uid="{1166767B-C3A8-6F47-B004-E3D9E1AAC2B9}" name="Navn"/>
     <tableColumn id="2" xr3:uid="{55BE3EDC-57A3-6042-915C-CBE889552E90}" name="Link"/>
     <tableColumn id="3" xr3:uid="{430447A9-979A-6F41-80F9-C1949336AD14}" name="Titel"/>
-    <tableColumn id="4" xr3:uid="{4E0B886A-F6FD-A242-AD55-C10C60DA5D47}" name="Stjerner" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{1C361871-60F3-1F46-935D-F813791A35C5}" name="Stikord" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{4E0B886A-F6FD-A242-AD55-C10C60DA5D47}" name="Stjerner" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{1C361871-60F3-1F46-935D-F813791A35C5}" name="Stikord" dataDxfId="0"/>
     <tableColumn id="8" xr3:uid="{14E1A955-0C73-6341-A5FB-F5576A2310C1}" name="# Citater"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -916,18 +1026,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42231D9-A03D-254A-930A-A47BD9C59C00}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="145.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="109.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="11" customWidth="1"/>
+    <col min="4" max="4" width="11" style="9" customWidth="1"/>
     <col min="5" max="5" width="110.6640625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -941,7 +1051,7 @@
       <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -961,7 +1071,7 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="9">
         <v>3</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -981,7 +1091,7 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="9">
         <v>5</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -1001,7 +1111,7 @@
       <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="9">
         <v>2</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -1021,7 +1131,7 @@
       <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="9">
         <v>2</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -1041,7 +1151,7 @@
       <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="9">
         <v>5</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -1061,7 +1171,7 @@
       <c r="C7" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="10">
         <v>5</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -1081,7 +1191,7 @@
       <c r="C8" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="9">
         <v>4</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -1101,7 +1211,7 @@
       <c r="C9" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="9">
         <v>1</v>
       </c>
       <c r="E9" s="4" t="s">
@@ -1121,7 +1231,7 @@
       <c r="C10" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="9">
         <v>1</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -1141,7 +1251,7 @@
       <c r="C11" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="9">
         <v>4</v>
       </c>
       <c r="E11" s="4" t="s">
@@ -1161,7 +1271,7 @@
       <c r="C12" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="9">
         <v>1</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -1181,7 +1291,7 @@
       <c r="C13" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="9">
         <v>4</v>
       </c>
       <c r="E13" s="4" t="s">
@@ -1201,7 +1311,7 @@
       <c r="C14" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="9">
         <v>1</v>
       </c>
       <c r="E14" s="4" t="s">
@@ -1221,7 +1331,7 @@
       <c r="C15" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="9">
         <v>1</v>
       </c>
       <c r="E15" s="4" t="s">
@@ -1241,7 +1351,7 @@
       <c r="C16" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="9">
         <v>1</v>
       </c>
       <c r="E16" s="4" t="s">
@@ -1261,7 +1371,7 @@
       <c r="C17" t="s">
         <v>68</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="9">
         <v>1</v>
       </c>
       <c r="E17" s="4" t="s">
@@ -1278,10 +1388,10 @@
       <c r="B18" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="9">
         <v>1</v>
       </c>
       <c r="E18" s="4" t="s">
@@ -1301,7 +1411,7 @@
       <c r="C19" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="9">
         <v>2</v>
       </c>
       <c r="E19" s="4" t="s">
@@ -1321,7 +1431,7 @@
       <c r="C20" t="s">
         <v>78</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20" s="10">
         <v>5</v>
       </c>
       <c r="E20" s="4" t="s">
@@ -1332,26 +1442,26 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D21" s="9">
         <v>2</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="6">
         <v>914</v>
       </c>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -1363,7 +1473,7 @@
       <c r="C22" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D22" s="9">
         <v>2</v>
       </c>
       <c r="E22" s="4" t="s">
@@ -1383,7 +1493,7 @@
       <c r="C23" t="s">
         <v>89</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="11">
         <v>4</v>
       </c>
       <c r="E23" s="4" t="s">
@@ -1403,7 +1513,7 @@
       <c r="C24" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="9">
         <v>5</v>
       </c>
       <c r="E24" s="4" t="s">
@@ -1414,22 +1524,22 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D25" s="12">
+      <c r="D25" s="10">
         <v>5</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="6">
         <v>497</v>
       </c>
     </row>
@@ -1443,7 +1553,7 @@
       <c r="C26" t="s">
         <v>101</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26" s="10">
         <v>5</v>
       </c>
       <c r="E26" s="4" t="s">
@@ -1463,7 +1573,7 @@
       <c r="C27" t="s">
         <v>104</v>
       </c>
-      <c r="D27" s="12">
+      <c r="D27" s="10">
         <v>5</v>
       </c>
       <c r="E27" s="4" t="s">
@@ -1474,7 +1584,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
+      <c r="A28" t="s">
         <v>111</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1483,7 +1593,7 @@
       <c r="C28" t="s">
         <v>108</v>
       </c>
-      <c r="D28" s="11">
+      <c r="D28" s="9">
         <v>3</v>
       </c>
       <c r="E28" s="4" t="s">
@@ -1494,16 +1604,16 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
+      <c r="A29" t="s">
         <v>112</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" t="s">
         <v>114</v>
       </c>
-      <c r="D29" s="11">
+      <c r="D29" s="9">
         <v>3</v>
       </c>
       <c r="E29" s="4" t="s">
@@ -1514,22 +1624,22 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D30" s="9">
         <v>5</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="6">
         <v>69009</v>
       </c>
     </row>
@@ -1540,10 +1650,10 @@
       <c r="B31" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" t="s">
         <v>123</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D31" s="9">
         <v>1</v>
       </c>
       <c r="E31" s="4" t="s">
@@ -1554,7 +1664,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
+      <c r="A32" t="s">
         <v>124</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1563,7 +1673,7 @@
       <c r="C32" t="s">
         <v>125</v>
       </c>
-      <c r="D32" s="11">
+      <c r="D32" s="9">
         <v>1</v>
       </c>
       <c r="E32" s="4" t="s">
@@ -1583,7 +1693,7 @@
       <c r="C33" t="s">
         <v>128</v>
       </c>
-      <c r="D33" s="11">
+      <c r="D33" s="9">
         <v>4</v>
       </c>
       <c r="E33" s="4" t="s">
@@ -1594,22 +1704,22 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="119" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="D34" s="11">
+      <c r="D34" s="9">
         <v>4</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E34" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="6">
         <v>9902</v>
       </c>
     </row>
@@ -1623,7 +1733,7 @@
       <c r="C35" t="s">
         <v>136</v>
       </c>
-      <c r="D35" s="11">
+      <c r="D35" s="9">
         <v>4</v>
       </c>
       <c r="E35" s="4" t="s">
@@ -1643,7 +1753,7 @@
       <c r="C36" t="s">
         <v>140</v>
       </c>
-      <c r="D36" s="13">
+      <c r="D36" s="11">
         <v>4</v>
       </c>
       <c r="E36" s="4" t="s">
@@ -1651,6 +1761,163 @@
       </c>
       <c r="F36">
         <v>1174</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>146</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C37" t="s">
+        <v>145</v>
+      </c>
+      <c r="D37" s="9">
+        <v>5</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F37">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A38" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D38" s="12">
+        <v>5</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="F38" s="6"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>155</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C39" t="s">
+        <v>151</v>
+      </c>
+      <c r="D39" s="9">
+        <v>5</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>158</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C40" t="s">
+        <v>156</v>
+      </c>
+      <c r="D40" s="9">
+        <v>5</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>163</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C41" t="s">
+        <v>162</v>
+      </c>
+      <c r="D41" s="9">
+        <v>5</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>167</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C42" t="s">
+        <v>166</v>
+      </c>
+      <c r="D42" s="9">
+        <v>5</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>170</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C43" t="s">
+        <v>169</v>
+      </c>
+      <c r="D43" s="9">
+        <v>5</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>173</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C44" t="s">
+        <v>172</v>
+      </c>
+      <c r="D44" s="9">
+        <v>5</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>179</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C45" t="s">
+        <v>177</v>
+      </c>
+      <c r="D45" s="9">
+        <v>4</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1690,10 +1957,19 @@
     <hyperlink ref="B36" r:id="rId33" xr:uid="{7BBC9801-BB86-804A-B00D-C0B096AAB344}"/>
     <hyperlink ref="B19" r:id="rId34" xr:uid="{F49D9848-C025-4E4B-8130-BF1458B8AB06}"/>
     <hyperlink ref="B33" r:id="rId35" xr:uid="{0FF38B02-4E7E-CD45-A6AB-35D62F26978B}"/>
+    <hyperlink ref="B37" r:id="rId36" xr:uid="{89ACA49C-777F-8B4B-A915-E3EE75D3C0B1}"/>
+    <hyperlink ref="B38" r:id="rId37" display="chrome-extension://efaidnbmnnnibpcajpcglclefindmkaj/https://www.researchgate.net/profile/Saba-Yahyaa/publication/276904847_Explorations_in_Reinforcement_Learning_Online_Action_Selection_and_Value_Function_Approximation/links/555b2ea408ae6943a8793fe3/Explorations-in-Reinforcement-Learning-Online-Action-Selection-and-Value-Function-Approximation.pdf" xr:uid="{7DDF338D-3B3A-4549-8E7D-E6760EEB1DCA}"/>
+    <hyperlink ref="B39" r:id="rId38" xr:uid="{D981D269-AD25-1C47-9F45-DE6E3C74753F}"/>
+    <hyperlink ref="B40" r:id="rId39" xr:uid="{3D6BD1EF-B637-3C43-8DD0-A23CACE4C99C}"/>
+    <hyperlink ref="B41" r:id="rId40" xr:uid="{2B981198-138E-D541-B629-E70943F7377B}"/>
+    <hyperlink ref="B42" r:id="rId41" xr:uid="{CFCADCD4-ADD8-2749-B91F-7EE50D870280}"/>
+    <hyperlink ref="B43" r:id="rId42" xr:uid="{31107A61-F4F5-8241-BF6E-D22E2EAE978A}"/>
+    <hyperlink ref="B44" r:id="rId43" xr:uid="{B8695455-2248-EE46-A727-56172CF0055C}"/>
+    <hyperlink ref="B45" r:id="rId44" xr:uid="{9FB98EDA-1073-2848-89FD-6835C29C8F4A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId36"/>
+    <tablePart r:id="rId45"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lørdag d. 23 marts kl.12
Lørdag d. 23 marts kl.12
</commit_message>
<xml_diff>
--- a/Liste over litteratur.xlsx
+++ b/Liste over litteratur.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Kirstine/Documents/GitHub/Bachelor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0186870C-82E5-1B41-845F-EE38214420A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249AF6D3-25DE-234C-A7A0-BB16587CD4EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{733265EB-9D21-354D-94CD-9E52C4EF0070}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="184">
   <si>
     <t>Navn</t>
   </si>
@@ -576,6 +576,18 @@
   </si>
   <si>
     <t>Yogeswaran &amp; Ponnambalam (2012)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fictitious Self-Play in Extensive-Form Games </t>
+  </si>
+  <si>
+    <t>http://proceedings.mlr.press/v37/heinrich15.pdf</t>
+  </si>
+  <si>
+    <t>Extensive-Form Fictitious Play</t>
+  </si>
+  <si>
+    <t>Heinrich et al. ()</t>
   </si>
 </sst>
 </file>
@@ -1026,10 +1038,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42231D9-A03D-254A-930A-A47BD9C59C00}">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1918,6 +1930,23 @@
       </c>
       <c r="E45" s="4" t="s">
         <v>178</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>183</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C46" t="s">
+        <v>180</v>
+      </c>
+      <c r="D46" s="9">
+        <v>5</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -1966,10 +1995,11 @@
     <hyperlink ref="B43" r:id="rId42" xr:uid="{31107A61-F4F5-8241-BF6E-D22E2EAE978A}"/>
     <hyperlink ref="B44" r:id="rId43" xr:uid="{B8695455-2248-EE46-A727-56172CF0055C}"/>
     <hyperlink ref="B45" r:id="rId44" xr:uid="{9FB98EDA-1073-2848-89FD-6835C29C8F4A}"/>
+    <hyperlink ref="B46" r:id="rId45" xr:uid="{C5ACFBE8-3A68-B74F-A09E-AE10897D2628}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId45"/>
+    <tablePart r:id="rId46"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>